<commit_message>
primara a produccion de modulo cotizacion proveedores
</commit_message>
<xml_diff>
--- a/public/assets/lte/descargas/Plantilla Listado Proveedor.xlsx
+++ b/public/assets/lte/descargas/Plantilla Listado Proveedor.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp.back\htdocs\ReportesBlueMix\public\assets\lte\descargas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>SKU Prov</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Categoria (OP)</t>
-  </si>
-  <si>
-    <t>Cotizado? (1-0)(OP)</t>
   </si>
 </sst>
 </file>
@@ -376,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1525"/>
+  <dimension ref="A1:G1524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,10 +387,9 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,53 +411,50 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
@@ -4987,9 +4980,6 @@
     </row>
     <row r="1524" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E1524"/>
-    </row>
-    <row r="1525" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E1525"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>